<commit_message>
Rename "beacon" to "oldBeacon" to prep for move
</commit_message>
<xml_diff>
--- a/test-data/sitewide-search.xlsx
+++ b/test-data/sitewide-search.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2D77DE8-5A36-4F6D-9F96-5133FCC1B7D1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1FD299CB-95F4-4F26-B753-AA9819525A16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SitewideSearch" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>argle-bargle</t>
   </si>
   <si>
-    <t xml:space="preserve"> Lorem ipsum dolor sit amet, consectetur adipiscing elit. Cras vitae neque consectetur, fringilla nunc eget, faucibus sem. Nulla aliquet imperdiet arcu, non dapibus lorem tincidunt pharetra. Donec sollicitudin risus sit amet eros facilisis eleifend. Donec</t>
-  </si>
-  <si>
     <t>CancerTerm</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>lanolina</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Cras vitae neque consectetur, fringilla nunc eget, faucibus sem. Nulla aliquet imperdiet arcu, non dapibus lorem tincidunt pharetra. Donec sollicitudin risus sit amet eros facilisis eleifend. Donec</t>
   </si>
 </sst>
 </file>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,19 +516,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -553,49 +553,49 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6634F395-7540-4542-954F-5DFBBE6DB702}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -626,66 +626,66 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted unneded methods from AnalyticsRequest
</commit_message>
<xml_diff>
--- a/test-data/sitewide-search.xlsx
+++ b/test-data/sitewide-search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F5C256A7-ABF6-4BE8-BE96-888FABB7C166}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4C058CFC-9064-448E-B003-57492DC15413}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,23 +26,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>breast</t>
   </si>
   <si>
-    <t>cancer</t>
-  </si>
-  <si>
     <t>ipilimumab</t>
   </si>
   <si>
     <t>Kaposi's sarcoma</t>
   </si>
   <si>
-    <t>shark</t>
-  </si>
-  <si>
     <t>CancerTerm</t>
   </si>
   <si>
@@ -70,21 +64,9 @@
     <t>10001110101 10001110101</t>
   </si>
   <si>
-    <t>Hematologic/Blood Cancers</t>
-  </si>
-  <si>
     <t xml:space="preserve">abdominoperineal resection </t>
   </si>
   <si>
-    <t>null allele</t>
-  </si>
-  <si>
-    <t>uninformative</t>
-  </si>
-  <si>
-    <t>lymphoma</t>
-  </si>
-  <si>
     <t>Dr. Norman E. Sharpless</t>
   </si>
   <si>
@@ -94,9 +76,6 @@
     <t>dolor</t>
   </si>
   <si>
-    <t>tabaco</t>
-  </si>
-  <si>
     <t>linfoma</t>
   </si>
   <si>
@@ -106,9 +85,6 @@
     <t>cáncer de hígado</t>
   </si>
   <si>
-    <t>A33</t>
-  </si>
-  <si>
     <t>safingol</t>
   </si>
   <si>
@@ -119,15 +95,6 @@
   </si>
   <si>
     <t>dermis</t>
-  </si>
-  <si>
-    <t>TAC-101</t>
-  </si>
-  <si>
-    <t>lanolina</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Cras vitae neque consectetur, fringilla nunc eget, faucibus sem. Nulla aliquet imperdiet arcu, non dapibus lorem tincidunt pharetra. Donec sollicitudin risus sit amet eros facilisis eleifend. Donec</t>
   </si>
   <si>
     <t>argle-bargle or foofaraw</t>
@@ -499,9 +466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -514,19 +483,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -534,72 +503,45 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>250</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2">
-        <v>250</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -609,10 +551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6634F395-7540-4542-954F-5DFBBE6DB702}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,66 +566,45 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>